<commit_message>
Fix snowman not returning to the same place when jumping
</commit_message>
<xml_diff>
--- a/Logbook.xlsx
+++ b/Logbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annet\Documents\GitHub\SnowScene\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1A4608-A848-4ED5-BFBB-B662288CCC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2043CAA-2D58-448C-B70D-9D139DB84417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31545" yWindow="2565" windowWidth="22890" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38505" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Time Spent</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Work on setting up scene</t>
   </si>
   <si>
-    <t>2 Hour</t>
-  </si>
-  <si>
     <t>Display the sky and ground on the screen. 3 ground points are random within a range. The sky has a gradient</t>
   </si>
   <si>
@@ -83,7 +80,31 @@
     <t>Created the Visual studio project with freeGlut set up. Worked out how to draw to the screen.</t>
   </si>
   <si>
-    <t>Draw Snowman features &amp; Snow</t>
+    <t>Draw Snow</t>
+  </si>
+  <si>
+    <t>Created particle system for display the snow</t>
+  </si>
+  <si>
+    <t>19/08/2024 1pm - 4pm</t>
+  </si>
+  <si>
+    <t>Add Features</t>
+  </si>
+  <si>
+    <t>20/08/2024 3pm - 5pm</t>
+  </si>
+  <si>
+    <t>3 Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fixed scaling system and the snow disappearing.  Display diagnostic data to the screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/08/2024 9am - </t>
+  </si>
+  <si>
+    <t>Added the ability for the snowman to jumping following a parabolic curve based on the time.</t>
   </si>
 </sst>
 </file>
@@ -413,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,43 +475,74 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>45523</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fade between day and night
</commit_message>
<xml_diff>
--- a/Logbook.xlsx
+++ b/Logbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annet\Documents\GitHub\SnowScene\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2043CAA-2D58-448C-B70D-9D139DB84417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA2805E-8943-4C9F-B689-5F443C7B2792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38505" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Time Spent</t>
   </si>
@@ -101,10 +101,19 @@
     <t xml:space="preserve"> Fixed scaling system and the snow disappearing.  Display diagnostic data to the screen</t>
   </si>
   <si>
-    <t xml:space="preserve">21/08/2024 9am - </t>
-  </si>
-  <si>
-    <t>Added the ability for the snowman to jumping following a parabolic curve based on the time.</t>
+    <t>21/08/2024 9am - 11am</t>
+  </si>
+  <si>
+    <t>Added the ability for the snowman to jumping following a parabolic curve based on the time. Fix the snowman not returning to the same place. Add day/night cycle</t>
+  </si>
+  <si>
+    <t>Add Features &amp; Diagnostic</t>
+  </si>
+  <si>
+    <t>I think I did well given the time spent. I unfortuanlly fell ill with influenza A which made it difficult to work on the proejct for a week and a half. Next time, I would make a start even earlier to ensure I had enough time to add the complex features that I wanted to add. I would also give the snowman more such as a scarf and t-shirt. While the snow might not be optimistise to handle large amounts of particles, I think I did well on managing what is still active and what is not.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When looking for two additional features to add, I thought back to what I had implemented in a previous Unity game. I decided on having the snowman jump when a key is pressed. There are lots of ways of doing this, but I decided on having the snowman follow a parabolic curve to add some kind of gravity effect like seen in the real world. I decided the best way to do this was to have the snowman snowballs be contained in an array so the values could be passed to the drawing function. For the 2nd feature, I decided on a daynight cycle as I thought it would add more to the scene.  I did think about having the snowman start to melt when the sun was out but decided that keeping track of the data needed to make it look good would be too complex. Instead, I had the sky fade between the two colour states for day and night. </t>
   </si>
 </sst>
 </file>
@@ -146,13 +155,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,18 +449,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="75" style="1" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -528,13 +543,16 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
@@ -545,8 +563,124 @@
         <v>22</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A8:D15"/>
+    <mergeCell ref="A18:D25"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>